<commit_message>
updated date ranges for raw data
</commit_message>
<xml_diff>
--- a/data/mating.disrupt.test.xlsx
+++ b/data/mating.disrupt.test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casper Crause\Documents\Keyphase\mating disruption\Research_project_pest_monitoring\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D54BF87-C774-4AE2-8D79-2AE32F96438F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FB5E8C-F385-4EA7-AF6A-A5140684A2AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B68DC978-E4B3-4F42-A0D5-064876B3E947}"/>
   </bookViews>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA0FE96-E9DC-4F94-9F24-C81E3B0CEADF}">
   <dimension ref="A4:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,11 +626,11 @@
         <v>11</v>
       </c>
       <c r="J8" s="1">
-        <v>43483</v>
+        <v>43634</v>
       </c>
       <c r="K8" s="1">
         <f>J8+90</f>
-        <v>43573</v>
+        <v>43724</v>
       </c>
       <c r="L8" t="s">
         <v>13</v>
@@ -661,11 +661,11 @@
         <v>11</v>
       </c>
       <c r="J9" s="1">
-        <v>43602</v>
+        <v>43831</v>
       </c>
       <c r="K9" s="1">
         <f>J9+90</f>
-        <v>43692</v>
+        <v>43921</v>
       </c>
       <c r="L9" t="s">
         <v>13</v>

</xml_diff>